<commit_message>
scraping and bracket added
</commit_message>
<xml_diff>
--- a/Men26Jun.xlsx
+++ b/Men26Jun.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="8555"/>
+    <workbookView windowWidth="23040" windowHeight="8555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
     <t>KAZ</t>
   </si>
   <si>
-    <t>QuadriARUNA</t>
+    <t>Quadri ARUNA</t>
   </si>
   <si>
     <t>Vicky WU</t>
@@ -1141,16 +1141,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1171,9 +1168,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1502,8 +1496,8 @@
   <sheetPr/>
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2833333333333" defaultRowHeight="13.8" outlineLevelCol="5"/>
@@ -1522,16 +1516,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1539,1468 +1533,1468 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="17.65" customHeight="1" spans="1:6">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="28.5" customHeight="1" spans="1:6">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7" t="s">
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="10" t="s">
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7" t="s">
+      <c r="D14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="D16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="D17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7" t="s">
+      <c r="D18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7" t="s">
+      <c r="D20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="D22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7" t="s">
+      <c r="D23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="7" t="s">
+      <c r="D24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="D25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="7" t="s">
+      <c r="D26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="11"/>
+      <c r="D27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="11" t="s">
+      <c r="D28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7" t="s">
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="7" t="s">
+      <c r="D30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="D31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="7" t="s">
+      <c r="D32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="7" t="s">
+      <c r="D33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="D34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="D35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7" t="s">
+      <c r="D36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="D37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7" t="s">
+      <c r="D38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="11"/>
+      <c r="D39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="11" t="s">
+      <c r="D40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7" t="s">
+      <c r="D41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7" t="s">
+      <c r="D42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
+      <c r="D43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="7" t="s">
+      <c r="D44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7" t="s">
+      <c r="D45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="46" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
+      <c r="D46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" ht="25" customHeight="1" spans="1:6">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7" t="s">
+      <c r="D47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="7" t="s">
+      <c r="D48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="49" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
+      <c r="D49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" ht="28.5" customHeight="1" spans="1:6">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="8"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="7" t="s">
+      <c r="D52" s="7"/>
+      <c r="E52" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="53" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="7" t="s">
+      <c r="D53" s="7"/>
+      <c r="E53" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="54" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="D54" s="7"/>
+      <c r="E54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="55" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" s="8"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="7" t="s">
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="57" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="7" t="s">
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="7" t="s">
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="59" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="7" t="s">
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="60" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="7" t="s">
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="61" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="7" t="s">
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="62" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="7" t="s">
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="63" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="7" t="s">
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="64" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="7" t="s">
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="65" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="7" t="s">
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="66" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="7" t="s">
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="67" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="7" t="s">
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="68" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="7" t="s">
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="69" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A69" s="4">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="7" t="s">
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="70" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="7" t="s">
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="71" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A71" s="4">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="7" t="s">
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="72" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="7" t="s">
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="73" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A73" s="4">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="7" t="s">
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="74" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="7" t="s">
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="75" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A75" s="4">
+      <c r="A75" s="3">
         <v>74</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="7" t="s">
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="76" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A76" s="4">
+      <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="7" t="s">
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="77" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A77" s="4">
+      <c r="A77" s="3">
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="7" t="s">
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="78" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A78" s="4">
+      <c r="A78" s="3">
         <v>77</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="7" t="s">
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="79" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A79" s="4">
+      <c r="A79" s="3">
         <v>78</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="7" t="s">
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="80" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A80" s="4">
+      <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="7" t="s">
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="81" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A81" s="4">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="7" t="s">
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="82" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A82" s="4">
+      <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="7" t="s">
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="83" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A83" s="4">
+      <c r="A83" s="3">
         <v>82</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="7" t="s">
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="84" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A84" s="4">
+      <c r="A84" s="3">
         <v>83</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="7" t="s">
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="85" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A85" s="4">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="7" t="s">
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="86" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A86" s="4">
+      <c r="A86" s="3">
         <v>85</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="7" t="s">
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="87" ht="16.5" customHeight="1" spans="1:6">
-      <c r="A87" s="4">
+      <c r="A87" s="3">
         <v>86</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="7" t="s">
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>